<commit_message>
feat: update config table0.9.0
</commit_message>
<xml_diff>
--- a/Excels/Area_区域表.xlsx
+++ b/Excels/Area_区域表.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>int</t>
   </si>
@@ -24,13 +24,19 @@
     <t>int[][]</t>
   </si>
   <si>
+    <t>boolean</t>
+  </si>
+  <si>
     <t>id</t>
   </si>
   <si>
     <t>name</t>
   </si>
   <si>
-    <t>range</t>
+    <t>points</t>
+  </si>
+  <si>
+    <t>isShape</t>
   </si>
   <si>
     <t xml:space="preserve">区域 ID</t>
@@ -39,7 +45,10 @@
     <t>名称</t>
   </si>
   <si>
-    <t>范围</t>
+    <t>点集</t>
+  </si>
+  <si>
+    <t>是否构成形状</t>
   </si>
   <si>
     <t>Language</t>
@@ -656,14 +665,14 @@
     <xf fontId="21" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf fontId="21" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf fontId="21" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1489,7 +1498,9 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2"/>
+      <c r="D1" s="4" t="s">
+        <v>3</v>
+      </c>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
@@ -1499,15 +1510,17 @@
     </row>
     <row r="2" s="2" customFormat="1">
       <c r="A2" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="2"/>
+      <c r="C2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>7</v>
+      </c>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
@@ -1517,15 +1530,17 @@
     </row>
     <row r="3" s="2" customFormat="1" ht="30">
       <c r="A3" s="2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>8</v>
+      <c r="C3" s="4" t="s">
+        <v>10</v>
       </c>
-      <c r="D3" s="2"/>
+      <c r="D3" s="4" t="s">
+        <v>11</v>
+      </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
@@ -1536,7 +1551,7 @@
     <row r="4" s="1" customFormat="1">
       <c r="A4" s="1"/>
       <c r="B4" s="1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -1548,14 +1563,14 @@
       <c r="J4" s="1"/>
     </row>
     <row r="5" s="1" customFormat="1" ht="30">
-      <c r="A5" s="4">
+      <c r="A5" s="5">
         <v>0</v>
       </c>
-      <c r="B5" s="5" t="s">
-        <v>10</v>
+      <c r="B5" s="6" t="s">
+        <v>13</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
@@ -1569,11 +1584,11 @@
       <c r="A6" s="1">
         <v>1</v>
       </c>
-      <c r="B6" s="5" t="s">
-        <v>12</v>
+      <c r="B6" s="6" t="s">
+        <v>15</v>
       </c>
-      <c r="C6" s="6" t="s">
-        <v>13</v>
+      <c r="C6" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
@@ -1584,8 +1599,8 @@
       <c r="J6" s="1"/>
     </row>
     <row r="7" s="1" customFormat="1" ht="30">
-      <c r="A7" s="4"/>
-      <c r="B7" s="5"/>
+      <c r="A7" s="5"/>
+      <c r="B7" s="6"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
@@ -1596,8 +1611,8 @@
       <c r="J7" s="1"/>
     </row>
     <row r="8" s="1" customFormat="1" ht="30">
-      <c r="A8" s="4"/>
-      <c r="B8" s="5"/>
+      <c r="A8" s="5"/>
+      <c r="B8" s="6"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
@@ -1621,7 +1636,7 @@
     </row>
     <row r="10" s="1" customFormat="1" ht="30">
       <c r="A10" s="1"/>
-      <c r="B10" s="5"/>
+      <c r="B10" s="6"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
@@ -1656,12 +1671,12 @@
     </row>
     <row r="13" s="1" customFormat="1">
       <c r="A13" s="1"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
@@ -1669,79 +1684,79 @@
     <row r="14" s="1" customFormat="1">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
     </row>
     <row r="15" s="1" customFormat="1">
       <c r="A15" s="1"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
     </row>
     <row r="16" s="1" customFormat="1">
       <c r="A16" s="1"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
     </row>
     <row r="17" s="1" customFormat="1">
       <c r="A17" s="1"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
     </row>
     <row r="18" s="1" customFormat="1">
       <c r="A18" s="1"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
     </row>
     <row r="19" s="1" customFormat="1">
       <c r="A19" s="7"/>
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
+      <c r="B19" s="6"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
     </row>
     <row r="20" s="1" customFormat="1">
       <c r="A20" s="7"/>
-      <c r="B20" s="5"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
@@ -1803,7 +1818,7 @@
     </row>
     <row r="26" s="1" customFormat="1">
       <c r="A26" s="7"/>
-      <c r="B26" s="5"/>
+      <c r="B26" s="6"/>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
@@ -1815,7 +1830,7 @@
     </row>
     <row r="27" s="1" customFormat="1">
       <c r="A27" s="7"/>
-      <c r="B27" s="5"/>
+      <c r="B27" s="6"/>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>

</xml_diff>

<commit_message>
feat: update Area config table
</commit_message>
<xml_diff>
--- a/Excels/Area_区域表.xlsx
+++ b/Excels/Area_区域表.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>int</t>
   </si>
@@ -22,9 +22,6 @@
   </si>
   <si>
     <t>int[][]</t>
-  </si>
-  <si>
-    <t>boolean</t>
   </si>
   <si>
     <t>id</t>
@@ -36,9 +33,6 @@
     <t>points</t>
   </si>
   <si>
-    <t>isShape</t>
-  </si>
-  <si>
     <t xml:space="preserve">区域 ID</t>
   </si>
   <si>
@@ -46,9 +40,6 @@
   </si>
   <si>
     <t>点集</t>
-  </si>
-  <si>
-    <t>是否构成形状</t>
   </si>
   <si>
     <t>Language</t>
@@ -665,14 +656,14 @@
     <xf fontId="21" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf fontId="21" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf fontId="21" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1484,8 +1475,8 @@
   <cols>
     <col min="1" max="1" style="0" width="10.875"/>
     <col customWidth="1" min="2" max="2" style="1" width="40.625"/>
-    <col customWidth="1" min="3" max="7" style="0" width="10.875"/>
-    <col min="8" max="16384" style="0" width="10.875"/>
+    <col customWidth="1" min="3" max="6" style="0" width="10.875"/>
+    <col min="7" max="16384" style="0" width="10.875"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="1">
@@ -1498,60 +1489,51 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
-        <v>3</v>
-      </c>
+      <c r="D1" s="2"/>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
     </row>
     <row r="2" s="2" customFormat="1">
       <c r="A2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>7</v>
-      </c>
+      <c r="D2" s="2"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
     </row>
     <row r="3" s="2" customFormat="1" ht="30">
       <c r="A3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>11</v>
-      </c>
+      <c r="D3" s="2"/>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
     </row>
     <row r="4" s="1" customFormat="1">
       <c r="A4" s="1"/>
       <c r="B4" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -1560,17 +1542,16 @@
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
     </row>
     <row r="5" s="1" customFormat="1" ht="30">
-      <c r="A5" s="5">
+      <c r="A5" s="4">
         <v>0</v>
       </c>
-      <c r="B5" s="6" t="s">
-        <v>13</v>
+      <c r="B5" s="5" t="s">
+        <v>10</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>14</v>
+      <c r="C5" s="6" t="s">
+        <v>11</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
@@ -1578,17 +1559,16 @@
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
     </row>
     <row r="6" s="1" customFormat="1" ht="30">
       <c r="A6" s="1">
         <v>1</v>
       </c>
-      <c r="B6" s="6" t="s">
-        <v>15</v>
+      <c r="B6" s="5" t="s">
+        <v>12</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
@@ -1596,11 +1576,10 @@
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
     </row>
     <row r="7" s="1" customFormat="1" ht="30">
-      <c r="A7" s="5"/>
-      <c r="B7" s="6"/>
+      <c r="A7" s="4"/>
+      <c r="B7" s="5"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
@@ -1608,11 +1587,10 @@
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
     </row>
     <row r="8" s="1" customFormat="1" ht="30">
-      <c r="A8" s="5"/>
-      <c r="B8" s="6"/>
+      <c r="A8" s="4"/>
+      <c r="B8" s="5"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
@@ -1620,7 +1598,6 @@
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
     </row>
     <row r="9" s="1" customFormat="1" ht="30">
       <c r="A9" s="1"/>
@@ -1632,11 +1609,10 @@
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
     </row>
     <row r="10" s="1" customFormat="1" ht="30">
       <c r="A10" s="1"/>
-      <c r="B10" s="6"/>
+      <c r="B10" s="5"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
@@ -1644,7 +1620,6 @@
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
     </row>
     <row r="11" s="1" customFormat="1">
       <c r="A11" s="1"/>
@@ -1656,7 +1631,6 @@
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
     </row>
     <row r="12" s="1" customFormat="1">
       <c r="A12" s="1"/>
@@ -1667,99 +1641,90 @@
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
-      <c r="J12" s="1"/>
     </row>
     <row r="13" s="1" customFormat="1">
       <c r="A13" s="1"/>
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="1"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
     </row>
     <row r="14" s="1" customFormat="1">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="1"/>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
-      <c r="J14" s="1"/>
     </row>
     <row r="15" s="1" customFormat="1">
       <c r="A15" s="1"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
-      <c r="G15" s="6"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="1"/>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
-      <c r="J15" s="1"/>
     </row>
     <row r="16" s="1" customFormat="1">
       <c r="A16" s="1"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="6"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="1"/>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
-      <c r="J16" s="1"/>
     </row>
     <row r="17" s="1" customFormat="1">
       <c r="A17" s="1"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="6"/>
-      <c r="G17" s="6"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="1"/>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
-      <c r="J17" s="1"/>
     </row>
     <row r="18" s="1" customFormat="1">
       <c r="A18" s="1"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="6"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="1"/>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
-      <c r="J18" s="1"/>
     </row>
     <row r="19" s="1" customFormat="1">
       <c r="A19" s="7"/>
-      <c r="B19" s="6"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="6"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="1"/>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
-      <c r="J19" s="1"/>
     </row>
     <row r="20" s="1" customFormat="1">
       <c r="A20" s="7"/>
-      <c r="B20" s="6"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="6"/>
-      <c r="G20" s="6"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="1"/>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
-      <c r="J20" s="1"/>
     </row>
     <row r="21" s="1" customFormat="1">
       <c r="A21" s="7"/>
@@ -1770,7 +1735,6 @@
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
-      <c r="J21" s="1"/>
     </row>
     <row r="22" s="1" customFormat="1">
       <c r="A22" s="7"/>
@@ -1781,7 +1745,6 @@
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
-      <c r="J22" s="1"/>
     </row>
     <row r="23" s="1" customFormat="1">
       <c r="A23" s="7"/>
@@ -1792,7 +1755,6 @@
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
-      <c r="J23" s="1"/>
     </row>
     <row r="24" s="1" customFormat="1">
       <c r="A24" s="7"/>
@@ -1803,7 +1765,6 @@
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
-      <c r="J24" s="1"/>
     </row>
     <row r="25" s="1" customFormat="1">
       <c r="A25" s="7"/>
@@ -1814,11 +1775,10 @@
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
-      <c r="J25" s="1"/>
     </row>
     <row r="26" s="1" customFormat="1">
       <c r="A26" s="7"/>
-      <c r="B26" s="6"/>
+      <c r="B26" s="5"/>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
@@ -1826,11 +1786,10 @@
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
-      <c r="J26" s="1"/>
     </row>
     <row r="27" s="1" customFormat="1">
       <c r="A27" s="7"/>
-      <c r="B27" s="6"/>
+      <c r="B27" s="5"/>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
@@ -1838,7 +1797,6 @@
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
-      <c r="J27" s="1"/>
     </row>
     <row r="28" s="1" customFormat="1">
       <c r="A28" s="7"/>
@@ -1849,7 +1807,6 @@
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
-      <c r="J28" s="1"/>
     </row>
     <row r="29" s="1" customFormat="1">
       <c r="A29" s="7"/>
@@ -1860,7 +1817,6 @@
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
-      <c r="J29" s="1"/>
     </row>
     <row r="30" s="1" customFormat="1">
       <c r="A30" s="7"/>
@@ -1871,7 +1827,6 @@
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
-      <c r="J30" s="1"/>
     </row>
     <row r="31" s="1" customFormat="1">
       <c r="A31" s="7"/>
@@ -1882,7 +1837,6 @@
       <c r="G31" s="1"/>
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
-      <c r="J31" s="1"/>
     </row>
     <row r="32" s="1" customFormat="1">
       <c r="A32" s="7"/>
@@ -1893,7 +1847,6 @@
       <c r="G32" s="1"/>
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
-      <c r="J32" s="1"/>
     </row>
     <row r="33" s="1" customFormat="1">
       <c r="A33" s="7"/>
@@ -1904,7 +1857,6 @@
       <c r="G33" s="1"/>
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
-      <c r="J33" s="1"/>
     </row>
     <row r="34" s="1" customFormat="1">
       <c r="A34" s="7"/>
@@ -1915,7 +1867,6 @@
       <c r="G34" s="1"/>
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
-      <c r="J34" s="1"/>
     </row>
     <row r="35" s="1" customFormat="1">
       <c r="A35" s="7"/>
@@ -1926,7 +1877,6 @@
       <c r="G35" s="1"/>
       <c r="H35" s="1"/>
       <c r="I35" s="1"/>
-      <c r="J35" s="1"/>
     </row>
     <row r="36" s="1" customFormat="1">
       <c r="A36" s="7"/>
@@ -1937,7 +1887,6 @@
       <c r="G36" s="1"/>
       <c r="H36" s="1"/>
       <c r="I36" s="1"/>
-      <c r="J36" s="1"/>
     </row>
     <row r="37" s="1" customFormat="1">
       <c r="A37" s="7"/>
@@ -1948,7 +1897,6 @@
       <c r="G37" s="1"/>
       <c r="H37" s="1"/>
       <c r="I37" s="1"/>
-      <c r="J37" s="1"/>
     </row>
     <row r="38" s="1" customFormat="1">
       <c r="A38" s="7"/>
@@ -1959,7 +1907,6 @@
       <c r="G38" s="1"/>
       <c r="H38" s="1"/>
       <c r="I38" s="1"/>
-      <c r="J38" s="1"/>
     </row>
     <row r="39" s="1" customFormat="1">
       <c r="A39" s="7"/>
@@ -1970,7 +1917,6 @@
       <c r="G39" s="1"/>
       <c r="H39" s="1"/>
       <c r="I39" s="1"/>
-      <c r="J39" s="1"/>
     </row>
     <row r="40" s="1" customFormat="1">
       <c r="A40" s="7"/>
@@ -1981,7 +1927,6 @@
       <c r="G40" s="1"/>
       <c r="H40" s="1"/>
       <c r="I40" s="1"/>
-      <c r="J40" s="1"/>
     </row>
     <row r="41" s="1" customFormat="1">
       <c r="A41" s="7"/>
@@ -1992,7 +1937,6 @@
       <c r="G41" s="1"/>
       <c r="H41" s="1"/>
       <c r="I41" s="1"/>
-      <c r="J41" s="1"/>
     </row>
     <row r="42" s="1" customFormat="1">
       <c r="A42" s="7"/>
@@ -2003,7 +1947,6 @@
       <c r="G42" s="1"/>
       <c r="H42" s="1"/>
       <c r="I42" s="1"/>
-      <c r="J42" s="1"/>
     </row>
     <row r="43" s="1" customFormat="1">
       <c r="A43" s="7"/>
@@ -2014,7 +1957,6 @@
       <c r="G43" s="1"/>
       <c r="H43" s="1"/>
       <c r="I43" s="1"/>
-      <c r="J43" s="1"/>
     </row>
     <row r="44" s="1" customFormat="1">
       <c r="A44" s="7"/>
@@ -2025,7 +1967,6 @@
       <c r="G44" s="1"/>
       <c r="H44" s="1"/>
       <c r="I44" s="1"/>
-      <c r="J44" s="1"/>
     </row>
     <row r="45" s="1" customFormat="1" ht="15">
       <c r="C45" s="1"/>
@@ -2035,7 +1976,6 @@
       <c r="G45" s="1"/>
       <c r="H45" s="1"/>
       <c r="I45" s="1"/>
-      <c r="J45" s="1"/>
     </row>
   </sheetData>
   <printOptions headings="0" gridLines="0"/>

</xml_diff>

<commit_message>
feat: update Area config
add birth point
</commit_message>
<xml_diff>
--- a/Excels/Area_区域表.xlsx
+++ b/Excels/Area_区域表.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>int</t>
   </si>
@@ -91,6 +91,12 @@
   </si>
   <si>
     <t>3006|-19105|1507||2716|-19680|1507||2716|-19680|1507||2722|-18470|1507||3026|-17945|1507||3876|-17945|1507</t>
+  </si>
+  <si>
+    <t>BirthPoint</t>
+  </si>
+  <si>
+    <t>3006|19105|1508</t>
   </si>
 </sst>
 </file>
@@ -148,11 +154,11 @@
     <xf fontId="0" fillId="0" borderId="0" numFmtId="49" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="49" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -211,7 +217,7 @@
           <color theme="4"/>
         </top>
         <bottom style="none"/>
-        <diagonal/>
+        <diagonal style="none"/>
       </border>
     </dxf>
     <dxf>
@@ -231,7 +237,7 @@
         <bottom style="thin">
           <color theme="4"/>
         </bottom>
-        <diagonal/>
+        <diagonal style="none"/>
         <horizontal style="thin">
           <color theme="4" tint="0.39994506668294322"/>
         </horizontal>
@@ -264,7 +270,7 @@
         <bottom style="thin">
           <color theme="4" tint="0.39994506668294322"/>
         </bottom>
-        <diagonal/>
+        <diagonal style="none"/>
       </border>
     </dxf>
     <dxf>
@@ -281,7 +287,7 @@
         <bottom style="thin">
           <color theme="4"/>
         </bottom>
-        <diagonal/>
+        <diagonal style="none"/>
       </border>
     </dxf>
     <dxf>
@@ -302,7 +308,7 @@
         <bottom style="thin">
           <color theme="4" tint="0.39994506668294322"/>
         </bottom>
-        <diagonal/>
+        <diagonal style="none"/>
       </border>
     </dxf>
     <dxf>
@@ -322,7 +328,7 @@
         <bottom style="thin">
           <color theme="4" tint="0.39994506668294322"/>
         </bottom>
-        <diagonal/>
+        <diagonal style="none"/>
       </border>
     </dxf>
     <dxf>
@@ -339,7 +345,7 @@
         <bottom style="thin">
           <color theme="4" tint="0.39994506668294322"/>
         </bottom>
-        <diagonal/>
+        <diagonal style="none"/>
       </border>
     </dxf>
     <dxf>
@@ -373,7 +379,7 @@
         <bottom style="thin">
           <color theme="4" tint="0.39994506668294322"/>
         </bottom>
-        <diagonal/>
+        <diagonal style="none"/>
       </border>
     </dxf>
   </dxfs>
@@ -1090,7 +1096,7 @@
       <c r="B16" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C16" s="7" t="s">
+      <c r="C16" s="5" t="s">
         <v>23</v>
       </c>
       <c r="D16" s="4"/>
@@ -1112,15 +1118,21 @@
       <c r="F17" s="4"/>
     </row>
     <row r="18" s="1" customFormat="1">
-      <c r="A18" s="8"/>
-      <c r="B18" s="4"/>
-      <c r="C18" s="4"/>
+      <c r="A18" s="7">
+        <v>14</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>27</v>
+      </c>
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
       <c r="F18" s="4"/>
     </row>
     <row r="19" s="1" customFormat="1">
-      <c r="A19" s="8"/>
+      <c r="A19" s="7"/>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
@@ -1128,78 +1140,78 @@
       <c r="F19" s="4"/>
     </row>
     <row r="20" s="1" customFormat="1">
-      <c r="A20" s="8"/>
+      <c r="A20" s="7"/>
     </row>
     <row r="21" s="1" customFormat="1">
-      <c r="A21" s="8"/>
+      <c r="A21" s="7"/>
     </row>
     <row r="22" s="1" customFormat="1">
-      <c r="A22" s="8"/>
+      <c r="A22" s="7"/>
     </row>
     <row r="23" s="1" customFormat="1">
-      <c r="A23" s="8"/>
+      <c r="A23" s="7"/>
     </row>
     <row r="24" s="1" customFormat="1">
-      <c r="A24" s="8"/>
+      <c r="A24" s="7"/>
     </row>
     <row r="25" s="1" customFormat="1">
-      <c r="A25" s="8"/>
+      <c r="A25" s="7"/>
       <c r="B25" s="4"/>
     </row>
     <row r="26" s="1" customFormat="1">
-      <c r="A26" s="8"/>
+      <c r="A26" s="7"/>
       <c r="B26" s="4"/>
     </row>
     <row r="27" s="1" customFormat="1">
-      <c r="A27" s="8"/>
+      <c r="A27" s="7"/>
     </row>
     <row r="28" s="1" customFormat="1">
-      <c r="A28" s="8"/>
+      <c r="A28" s="7"/>
     </row>
     <row r="29" s="1" customFormat="1">
-      <c r="A29" s="8"/>
+      <c r="A29" s="7"/>
     </row>
     <row r="30" s="1" customFormat="1">
-      <c r="A30" s="8"/>
+      <c r="A30" s="7"/>
     </row>
     <row r="31" s="1" customFormat="1">
-      <c r="A31" s="8"/>
+      <c r="A31" s="7"/>
     </row>
     <row r="32" s="1" customFormat="1">
-      <c r="A32" s="8"/>
+      <c r="A32" s="7"/>
     </row>
     <row r="33" s="1" customFormat="1">
-      <c r="A33" s="8"/>
+      <c r="A33" s="7"/>
     </row>
     <row r="34" s="1" customFormat="1">
-      <c r="A34" s="8"/>
+      <c r="A34" s="7"/>
     </row>
     <row r="35" s="1" customFormat="1">
-      <c r="A35" s="8"/>
+      <c r="A35" s="7"/>
     </row>
     <row r="36" s="1" customFormat="1">
-      <c r="A36" s="8"/>
+      <c r="A36" s="7"/>
     </row>
     <row r="37" s="1" customFormat="1">
-      <c r="A37" s="8"/>
+      <c r="A37" s="7"/>
     </row>
     <row r="38" s="1" customFormat="1">
-      <c r="A38" s="8"/>
+      <c r="A38" s="7"/>
     </row>
     <row r="39" s="1" customFormat="1">
-      <c r="A39" s="8"/>
+      <c r="A39" s="7"/>
     </row>
     <row r="40" s="1" customFormat="1">
-      <c r="A40" s="8"/>
+      <c r="A40" s="7"/>
     </row>
     <row r="41" s="1" customFormat="1">
-      <c r="A41" s="8"/>
+      <c r="A41" s="7"/>
     </row>
     <row r="42" s="1" customFormat="1">
-      <c r="A42" s="8"/>
+      <c r="A42" s="7"/>
     </row>
     <row r="43" s="1" customFormat="1">
-      <c r="A43" s="8"/>
+      <c r="A43" s="7"/>
     </row>
     <row r="44" s="1" customFormat="1"/>
   </sheetData>

</xml_diff>

<commit_message>
feat: update MainPanel UI
修改主界面UI按钮位置；
修改场景龙生成区域
</commit_message>
<xml_diff>
--- a/Excels/Area_区域表.xlsx
+++ b/Excels/Area_区域表.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\MetaApp\Editor_Win64\MetaWorldSaved\Saved\MetaWorld\Project\Edit\DragonVerse\Excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B172AF25-27FB-4EBD-9910-4111705FE647}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{290E3412-8E42-4BBD-8D13-89D691BE2C66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -101,19 +101,19 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>-2673|-11203|430||-2835|-10598|430||-3227|-10666|392</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>-2461|-11936|480||-2673|-11203|430||-1908|-12482|530</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>-3090|-6200|990||-3533|-5161|1131||-4460|-3301|1337||-4038|-5173|1202</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>-858|-7036|714||-2389|-8190|940||-3963|-7967|1011</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>-2461|-11936|480||-2673|-11203|440||-1908|-12482|530</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>-2673|-11203|440||-2835|-10598|440||-3227|-10666|3400</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -655,7 +655,7 @@
   <dimension ref="A1:F44"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="16.5" x14ac:dyDescent="0.35"/>
@@ -722,7 +722,7 @@
         <v>10</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.35">
@@ -733,7 +733,7 @@
         <v>10</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.35">
@@ -755,7 +755,7 @@
         <v>10</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.35">
@@ -766,7 +766,7 @@
         <v>10</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.35">

</xml_diff>